<commit_message>
Updated Funds Input data till 14-Nov
</commit_message>
<xml_diff>
--- a/fund.xlsx
+++ b/fund.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Daily" sheetId="1" r:id="rId1"/>
+    <sheet name="Fund" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Total</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>Input</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -384,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -572,12 +575,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" s="4" customFormat="1">
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="1">
+        <v>43019</v>
+      </c>
+      <c r="D4">
+        <v>101</v>
+      </c>
+      <c r="H4">
+        <f>D4</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="1">
+        <v>43019</v>
+      </c>
+      <c r="D5">
+        <v>50000</v>
+      </c>
+      <c r="H5">
+        <f>H4+D5-F5</f>
+        <v>50101</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" s="1">
+        <v>43020</v>
+      </c>
+      <c r="D6">
+        <v>50000</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H9" si="0">H5+D6-F6</f>
+        <v>100101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" s="1">
+        <v>43040</v>
+      </c>
+      <c r="D7">
+        <v>20000</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>120101</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="1">
+        <v>43045</v>
+      </c>
+      <c r="D8">
+        <v>75000</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>195101</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="1">
+        <v>43052</v>
+      </c>
+      <c r="D9">
+        <v>35000</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>230101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated funds and net upto 27-Nov
</commit_message>
<xml_diff>
--- a/fund.xlsx
+++ b/fund.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Total</t>
   </si>
@@ -34,6 +34,24 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Pts</t>
+  </si>
+  <si>
+    <t>Amt</t>
+  </si>
+  <si>
+    <t>Pay In</t>
+  </si>
+  <si>
+    <t>Cur</t>
   </si>
 </sst>
 </file>
@@ -385,14 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:K15"/>
+  <dimension ref="A2:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="9" max="9" width="12" style="4" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" style="4" customWidth="1"/>
   </cols>
@@ -429,8 +448,8 @@
         <v>101</v>
       </c>
       <c r="K4" s="4">
-        <f>SUM(B4:B24)</f>
-        <v>100101</v>
+        <f>SUM(B4:B25)</f>
+        <v>145101</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -566,6 +585,94 @@
         <v>92731.11</v>
       </c>
       <c r="K15" s="6"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="G17">
+        <v>250212.79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>43059</v>
+      </c>
+      <c r="D18">
+        <v>3917.99</v>
+      </c>
+      <c r="G18">
+        <f>G17-D18+E18</f>
+        <v>246294.80000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1">
+        <v>43060</v>
+      </c>
+      <c r="D19">
+        <v>3480</v>
+      </c>
+      <c r="G19">
+        <f>G18-D19+E19</f>
+        <v>242814.80000000002</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1">
+        <v>43063</v>
+      </c>
+      <c r="D20">
+        <v>1761</v>
+      </c>
+      <c r="G20">
+        <f>G19-D20+E20</f>
+        <v>241053.80000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1">
+        <v>43066</v>
+      </c>
+      <c r="B21">
+        <v>45000</v>
+      </c>
+      <c r="G21">
+        <f>G20+B21-D21+E21</f>
+        <v>286053.80000000005</v>
+      </c>
+      <c r="I21" s="5">
+        <v>286052.25</v>
+      </c>
+      <c r="K21" s="5">
+        <v>275101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1">
+        <v>43066</v>
+      </c>
+      <c r="E23">
+        <v>6700</v>
+      </c>
+      <c r="G23">
+        <f>I21+E23</f>
+        <v>292752.25</v>
+      </c>
+      <c r="K23" s="4">
+        <f>G23-K21</f>
+        <v>17651.25</v>
+      </c>
+      <c r="M23">
+        <f>K23/75</f>
+        <v>235.35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,10 +682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H9"/>
+  <dimension ref="B2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -635,7 +742,7 @@
         <v>50000</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H9" si="0">H5+D6-F6</f>
+        <f t="shared" ref="H6:H8" si="0">H5+D6-F6</f>
         <v>100101</v>
       </c>
     </row>
@@ -671,8 +778,20 @@
         <v>35000</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>H8+D9-F9</f>
         <v>230101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="1">
+        <v>43066</v>
+      </c>
+      <c r="D10">
+        <v>45000</v>
+      </c>
+      <c r="H10">
+        <f>H9+D10-F10</f>
+        <v>275101</v>
       </c>
     </row>
   </sheetData>
@@ -682,12 +801,80 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="3:9" s="5" customFormat="1">
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9">
+      <c r="C3">
+        <v>32.15</v>
+      </c>
+      <c r="E3">
+        <v>109.95</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9">
+      <c r="C4">
+        <v>35.15</v>
+      </c>
+      <c r="E4">
+        <v>113.65</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9">
+      <c r="C5">
+        <v>170.15</v>
+      </c>
+      <c r="E5">
+        <v>46.95</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9">
+      <c r="C6">
+        <v>31.15</v>
+      </c>
+      <c r="E6">
+        <v>88.95</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9">
+      <c r="C8">
+        <f>SUM(C3:C6)</f>
+        <v>268.59999999999997</v>
+      </c>
+      <c r="E8">
+        <f>SUM(E3:E6)</f>
+        <v>359.5</v>
+      </c>
+      <c r="G8">
+        <f>E8-C8</f>
+        <v>90.900000000000034</v>
+      </c>
+      <c r="I8">
+        <f>G8*75</f>
+        <v>6817.5000000000027</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>